<commit_message>
Updated sprint product owner
</commit_message>
<xml_diff>
--- a/sprint-backlogs/Sprint 1.xlsx
+++ b/sprint-backlogs/Sprint 1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40e7275a791a35e0/Documents/Team213/sprint-backlogs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Classes\Web App Development\Team213\sprint-backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -179,9 +179,6 @@
     <t>Caleb De la Cruz (cdelacru)</t>
   </si>
   <si>
-    <t>Abishek Anand (asanand)</t>
-  </si>
-  <si>
     <t>Hours</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>https://trello.com/b/5tEQHZBy</t>
+  </si>
+  <si>
+    <t>Abishek Anand (asanand) - Product Owner</t>
   </si>
 </sst>
 </file>
@@ -643,7 +643,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,17 +656,17 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -923,7 +923,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -935,7 +935,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -943,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -951,7 +951,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -959,7 +959,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -967,7 +967,7 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -975,7 +975,7 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>